<commit_message>
Correções em visual do excel
</commit_message>
<xml_diff>
--- a/Logs.xlsx
+++ b/Logs.xlsx
@@ -31,19 +31,10 @@
     <t>GET</t>
   </si>
   <si>
-    <t>product inserted directly into the database</t>
-  </si>
-  <si>
-    <t>2022-12-14 00:18:50</t>
-  </si>
-  <si>
     <t>user 'admin' gets all products from database</t>
   </si>
   <si>
-    <t>2022-12-14 00:40:25</t>
-  </si>
-  <si>
-    <t>2022-12-14 00:40:33</t>
+    <t>2022-12-14 09:25:06</t>
   </si>
   <si>
     <t>POST</t>
@@ -52,10 +43,13 @@
     <t>user 'admin' inserted product '4' from database</t>
   </si>
   <si>
+    <t>2022-12-14 09:25:13</t>
+  </si>
+  <si>
     <t>user 'admin' gets product '4' from database</t>
   </si>
   <si>
-    <t>2022-12-14 00:40:35</t>
+    <t>2022-12-14 09:25:18</t>
   </si>
   <si>
     <t>PUT</t>
@@ -64,7 +58,13 @@
     <t>user 'admin' updated product '4' from database</t>
   </si>
   <si>
-    <t>2022-12-14 00:40:37</t>
+    <t>2022-12-14 09:25:21</t>
+  </si>
+  <si>
+    <t>2022-12-14 09:25:22</t>
+  </si>
+  <si>
+    <t>2022-12-14 09:25:25</t>
   </si>
   <si>
     <t>DELETE</t>
@@ -73,7 +73,7 @@
     <t>user 'admin' deleted product '4' from database</t>
   </si>
   <si>
-    <t>2022-12-14 00:40:39</t>
+    <t>2022-12-14 09:25:27</t>
   </si>
 </sst>
 </file>
@@ -95,24 +95,28 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="1"/>
       <sz val="11"/>
-      <color rgb="FF00FFFF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="1"/>
       <sz val="11"/>
-      <color rgb="FF00FF7F"/>
+      <color rgb="FF006400"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="1"/>
       <sz val="11"/>
-      <color rgb="FFEE82EE"/>
+      <color rgb="FF003399"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FFB22222"/>
       <name val="Calibri"/>
@@ -133,7 +137,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,17 +491,17 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -508,10 +512,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -522,10 +526,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -536,24 +540,24 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -564,10 +568,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -578,10 +582,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -592,10 +596,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -603,10 +607,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>16</v>
@@ -620,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
@@ -634,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>16</v>
@@ -662,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>19</v>

</xml_diff>